<commit_message>
Added average on figure1.xlsx.
</commit_message>
<xml_diff>
--- a/paper/pldi21/img/figure1.xlsx
+++ b/paper/pldi21/img/figure1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonyoungpark/Work/safe/paper/pldi21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFC2459-AC2B-344D-9735-41188A23B1AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC3BE3-5FEF-5B4C-B7F2-F164FE793C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="51200" windowHeight="26660" xr2:uid="{8A9D149F-BF0C-F247-A8AE-6DB769120710}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26660" xr2:uid="{8A9D149F-BF0C-F247-A8AE-6DB769120710}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 1 (2)" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Benchmark</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,6 +191,10 @@
   </si>
   <si>
     <t>[-213][-118][-145][-150][-143][-131][-132][-169][-112][-212][-225][-144]</t>
+  </si>
+  <si>
+    <t>Time ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1303,8 +1307,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>963614</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>20484</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1636,10 +1640,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A4B56D-DF95-BE49-8C94-9C8311EBA243}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1655,7 +1659,7 @@
     <col min="10" max="10" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1695,8 +1699,11 @@
       <c r="M1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1732,8 +1739,12 @@
         <f>K2/1000</f>
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1">
+      <c r="N2">
+        <f>L2/M2</f>
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" hidden="1">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1744,7 +1755,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:14" hidden="1">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1755,7 +1766,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:14" hidden="1">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1792,7 +1803,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1828,8 +1839,12 @@
         <f t="shared" si="1"/>
         <v>0.30499999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <f t="shared" ref="N6:N11" si="2">L6/M6</f>
+        <v>3.4098360655737707</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1862,8 +1877,12 @@
         <f t="shared" si="1"/>
         <v>0.183</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>3.043715846994536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1896,8 +1915,12 @@
         <f t="shared" si="1"/>
         <v>0.41899999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>8.4868735083532219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1930,8 +1953,12 @@
         <f t="shared" si="1"/>
         <v>0.191</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>0.42408376963350786</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1967,8 +1994,12 @@
         <f t="shared" si="1"/>
         <v>0.34499999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>1.173913043478261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2001,8 +2032,12 @@
         <f t="shared" si="1"/>
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" hidden="1">
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>8.3673469387755102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" hidden="1">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2013,7 +2048,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1">
+    <row r="13" spans="1:14" hidden="1">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2024,7 +2059,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1">
+    <row r="14" spans="1:14" hidden="1">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2035,7 +2070,7 @@
         <v>2435</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2064,15 +2099,19 @@
         <v>315</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L18" si="2">E15/1000</f>
+        <f t="shared" ref="L15:L18" si="3">E15/1000</f>
         <v>0.40300000000000002</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M18" si="3">K15/1000</f>
+        <f t="shared" ref="M15:M18" si="4">K15/1000</f>
         <v>0.315</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15">
+        <f t="shared" ref="N15:N16" si="5">L15/M15</f>
+        <v>1.2793650793650795</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2101,15 +2140,19 @@
         <v>226</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.73299999999999998</v>
       </c>
       <c r="M16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22600000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" hidden="1">
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>3.2433628318584069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" hidden="1">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2138,15 +2181,15 @@
         <v>194</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42.283000000000001</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2175,15 +2218,19 @@
         <v>1949</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.97</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9490000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1">
+      <c r="N18">
+        <f>L18/M18</f>
+        <v>3.5761929194458695</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" hidden="1">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2194,7 +2241,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1">
+    <row r="20" spans="1:14" hidden="1">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2205,7 +2252,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1">
+    <row r="21" spans="1:14" hidden="1">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -2242,7 +2289,7 @@
         <v>0.11799999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1">
+    <row r="22" spans="1:14" hidden="1">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2253,7 +2300,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1">
+    <row r="23" spans="1:14" hidden="1">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2288,6 +2335,62 @@
       <c r="M23">
         <f>K23/1000</f>
         <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="N26">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="N27">
+        <v>3.4098360655737707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="N28">
+        <v>3.043715846994536</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="N29">
+        <v>8.4868735083532219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="N30">
+        <v>0.42408376963350786</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="N31">
+        <v>1.173913043478261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="N32">
+        <v>8.3673469387755102</v>
+      </c>
+    </row>
+    <row r="33" spans="14:14">
+      <c r="N33">
+        <v>1.2793650793650795</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14">
+      <c r="N34">
+        <v>3.2433628318584069</v>
+      </c>
+    </row>
+    <row r="35" spans="14:14">
+      <c r="N35">
+        <v>3.5761929194458695</v>
+      </c>
+    </row>
+    <row r="36" spans="14:14">
+      <c r="N36">
+        <f>AVERAGE(N26:N35)</f>
+        <v>4.7254690003478164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Figure 1 to SunSpider.
</commit_message>
<xml_diff>
--- a/paper/pldi21/img/figure1.xlsx
+++ b/paper/pldi21/img/figure1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonyoungpark/Work/safe/paper/pldi21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC3BE3-5FEF-5B4C-B7F2-F164FE793C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3782834F-0DF4-5044-890E-0803F71EF689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26660" xr2:uid="{8A9D149F-BF0C-F247-A8AE-6DB769120710}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Figure 1 (2)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Figure 1 (2)'!$A$1:$K$23</definedName>
-    <definedName name="summary" localSheetId="0">'Figure 1 (2)'!$A$1:$J$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Figure 1 (2)'!$A$1:$O$23</definedName>
+    <definedName name="summary" localSheetId="0">'Figure 1 (2)'!$B$1:$K$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Benchmark</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -194,6 +194,21 @@
   </si>
   <si>
     <t>Time ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v8_v7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SunSpider</t>
+  </si>
+  <si>
+    <t>SunSpider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -201,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -213,6 +228,14 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -237,8 +260,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -292,7 +316,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Figure 1 (2)'!$L$1</c:f>
+              <c:f>'Figure 1 (2)'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -313,77 +337,89 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Figure 1 (2)'!$A$2:$A$23</c:f>
+              <c:f>'Figure 1 (2)'!$B$2:$B$23</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3d-morph</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>access-nbody</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>access-nsieve</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>bitops-3bit-bits-in-byte</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>bitops-bits-in-byte</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>bitops-bitwise-and</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>bitops-nsieve-bits</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>controlflow-recursive</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>math-cordic</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>math-partial-sums</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>navier-stokes</c:v>
+                <c:pt idx="10">
+                  <c:v>math-spectral-norm</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>string-fasta</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 1 (2)'!$L$2:$L$23</c:f>
+              <c:f>'Figure 1 (2)'!$M$2:$M$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>4.1609999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>27.236999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.04</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.55700000000000005</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3.556</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>8.1000000000000003E-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.40500000000000003</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.64</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.40300000000000002</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.73299999999999998</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.97</c:v>
+                <c:pt idx="10">
+                  <c:v>42.283000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,7 +435,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Figure 1 (2)'!$M$1</c:f>
+              <c:f>'Figure 1 (2)'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -420,77 +456,89 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Figure 1 (2)'!$A$2:$A$23</c:f>
+              <c:f>'Figure 1 (2)'!$B$2:$B$23</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3d-morph</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>access-nbody</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>access-nsieve</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>bitops-3bit-bits-in-byte</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>bitops-bits-in-byte</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>bitops-bitwise-and</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>bitops-nsieve-bits</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>controlflow-recursive</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>math-cordic</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>math-partial-sums</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>navier-stokes</c:v>
+                <c:pt idx="10">
+                  <c:v>math-spectral-norm</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>string-fasta</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 1 (2)'!$M$2:$M$23</c:f>
+              <c:f>'Figure 1 (2)'!$N$2:$N$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.29199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.245</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.30499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.183</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.41899999999999998</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.191</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.34499999999999997</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.19600000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.315</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.22600000000000001</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.9490000000000001</c:v>
+                <c:pt idx="10">
+                  <c:v>0.19400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25700000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,7 +610,6 @@
         <c:axId val="944746960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1299,16 +1346,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>485306</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>40226</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>423853</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>153628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>963614</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>20484</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4291371</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>122903</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1640,774 +1687,865 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A4B56D-DF95-BE49-8C94-9C8311EBA243}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>4161</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>292</v>
       </c>
-      <c r="L2">
-        <f>E2/1000</f>
+      <c r="M2">
+        <f>F2/1000</f>
         <v>4.1609999999999996</v>
       </c>
-      <c r="M2">
-        <f>K2/1000</f>
+      <c r="N2">
+        <f>L2/1000</f>
         <v>0.29199999999999998</v>
       </c>
-      <c r="N2">
-        <f>L2/M2</f>
+      <c r="O2">
+        <f>M2/N2</f>
         <v>14.25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1">
+    <row r="3" spans="1:15" hidden="1">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" hidden="1">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>707</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>27237</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>245</v>
       </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L11" si="0">E5/1000</f>
+      <c r="M5">
+        <f t="shared" ref="M5:M11" si="0">F5/1000</f>
         <v>27.236999999999998</v>
       </c>
-      <c r="M5">
-        <f t="shared" ref="M5:M11" si="1">K5/1000</f>
+      <c r="N5">
+        <f t="shared" ref="N5:N11" si="1">L5/1000</f>
         <v>0.245</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
+      <c r="O5">
+        <f t="shared" ref="O5:O11" si="2">M5/N5</f>
+        <v>111.17142857142856</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>1040</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>21</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>305</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f t="shared" si="1"/>
         <v>0.30499999999999999</v>
       </c>
-      <c r="N6">
-        <f t="shared" ref="N6:N11" si="2">L6/M6</f>
+      <c r="O6">
+        <f t="shared" si="2"/>
         <v>3.4098360655737707</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>557</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>183</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>0.55700000000000005</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="1"/>
         <v>0.183</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f t="shared" si="2"/>
         <v>3.043715846994536</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>3556</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>8</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>419</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>3.556</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="1"/>
         <v>0.41899999999999998</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f t="shared" si="2"/>
         <v>8.4868735083532219</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>81</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>191</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="1"/>
         <v>0.191</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f t="shared" si="2"/>
         <v>0.42408376963350786</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>405</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>10</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>26</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>345</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="0"/>
         <v>0.40500000000000003</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <f t="shared" si="1"/>
         <v>0.34499999999999997</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <f t="shared" si="2"/>
         <v>1.173913043478261</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>1640</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>196</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f t="shared" si="1"/>
         <v>0.19600000000000001</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <f t="shared" si="2"/>
         <v>8.3673469387755102</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1">
-      <c r="A12" t="s">
+    <row r="12" spans="1:15" hidden="1">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>1059</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1">
+    <row r="13" spans="1:15" hidden="1">
       <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1">
+    <row r="14" spans="1:15" hidden="1">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>2435</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>403</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>1</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>6</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>32</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>315</v>
       </c>
-      <c r="L15">
-        <f t="shared" ref="L15:L18" si="3">E15/1000</f>
+      <c r="M15">
+        <f t="shared" ref="M15:M18" si="3">F15/1000</f>
         <v>0.40300000000000002</v>
       </c>
-      <c r="M15">
-        <f t="shared" ref="M15:M18" si="4">K15/1000</f>
+      <c r="N15">
+        <f t="shared" ref="N15:N18" si="4">L15/1000</f>
         <v>0.315</v>
       </c>
-      <c r="N15">
-        <f t="shared" ref="N15:N16" si="5">L15/M15</f>
+      <c r="O15">
+        <f t="shared" ref="O15:O18" si="5">M15/N15</f>
         <v>1.2793650793650795</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" t="s">
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>733</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>4</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>34</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>226</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f t="shared" si="3"/>
         <v>0.73299999999999998</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <f t="shared" si="4"/>
         <v>0.22600000000000001</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <f t="shared" si="5"/>
         <v>3.2433628318584069</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1">
-      <c r="A17" t="s">
+    <row r="17" spans="1:15">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>42283</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>16</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>36</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>194</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="3"/>
         <v>42.283000000000001</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <f t="shared" si="4"/>
         <v>0.19400000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17">
+        <f t="shared" si="5"/>
+        <v>217.95360824742269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" hidden="1">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>6970</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>1</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>77</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>38</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>1949</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f t="shared" si="3"/>
         <v>6.97</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <f t="shared" si="4"/>
         <v>1.9490000000000001</v>
       </c>
-      <c r="N18">
-        <f>L18/M18</f>
+      <c r="O18">
+        <f t="shared" si="5"/>
         <v>3.5761929194458695</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1">
+    <row r="19" spans="1:15" hidden="1">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>424</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1">
+    <row r="20" spans="1:15" hidden="1">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1">
+    <row r="21" spans="1:15" hidden="1">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="E21">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>29781</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>56</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>42</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>118</v>
       </c>
-      <c r="L21">
-        <f>E21/1000</f>
+      <c r="M21">
+        <f>F21/1000</f>
         <v>29.780999999999999</v>
       </c>
-      <c r="M21">
-        <f>K21/1000</f>
+      <c r="N21">
+        <f>L21/1000</f>
         <v>0.11799999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" hidden="1">
+      <c r="O21">
+        <f>M21/N21</f>
+        <v>252.38135593220341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" hidden="1">
       <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>1031</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1">
-      <c r="A23" t="s">
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="E23">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>11596</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>16</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>45</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>257</v>
       </c>
-      <c r="L23">
-        <f>E23/1000</f>
+      <c r="M23">
+        <f>F23/1000</f>
         <v>11.596</v>
       </c>
-      <c r="M23">
-        <f>K23/1000</f>
+      <c r="N23">
+        <f>L23/1000</f>
         <v>0.25700000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="N26">
+      <c r="O23">
+        <f>M23/N23</f>
+        <v>45.120622568093381</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="O26">
         <v>14.25</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
-      <c r="N27">
+    <row r="27" spans="1:15">
+      <c r="O27">
+        <v>111.17142857142856</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="O28">
         <v>3.4098360655737707</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
-      <c r="N28">
+    <row r="29" spans="1:15">
+      <c r="O29">
         <v>3.043715846994536</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
-      <c r="N29">
+    <row r="30" spans="1:15">
+      <c r="O30">
         <v>8.4868735083532219</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
-      <c r="N30">
+    <row r="31" spans="1:15">
+      <c r="O31">
         <v>0.42408376963350786</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
-      <c r="N31">
+    <row r="32" spans="1:15">
+      <c r="O32">
         <v>1.173913043478261</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
-      <c r="N32">
+    <row r="33" spans="15:15">
+      <c r="O33">
         <v>8.3673469387755102</v>
       </c>
     </row>
-    <row r="33" spans="14:14">
-      <c r="N33">
+    <row r="34" spans="15:15">
+      <c r="O34">
         <v>1.2793650793650795</v>
       </c>
     </row>
-    <row r="34" spans="14:14">
-      <c r="N34">
+    <row r="35" spans="15:15">
+      <c r="O35">
         <v>3.2433628318584069</v>
       </c>
     </row>
-    <row r="35" spans="14:14">
-      <c r="N35">
-        <v>3.5761929194458695</v>
-      </c>
-    </row>
-    <row r="36" spans="14:14">
-      <c r="N36">
-        <f>AVERAGE(N26:N35)</f>
-        <v>4.7254690003478164</v>
+    <row r="36" spans="15:15">
+      <c r="O36">
+        <v>217.95360824742269</v>
+      </c>
+    </row>
+    <row r="37" spans="15:15">
+      <c r="O37">
+        <v>45.120622568093381</v>
+      </c>
+    </row>
+    <row r="39" spans="15:15">
+      <c r="O39">
+        <f>AVERAGE(O26:O37)</f>
+        <v>34.827013039248079</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K23" xr:uid="{7510BFC1-4192-174F-BAA6-B537FE8A3DDE}">
-    <filterColumn colId="4">
+  <autoFilter ref="A1:O23" xr:uid="{F6419CC3-5AAD-B843-9EC1-DBE108C9CE82}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="1040"/>
-        <filter val="1640"/>
-        <filter val="3556"/>
-        <filter val="403"/>
-        <filter val="405"/>
-        <filter val="4161"/>
-        <filter val="557"/>
-        <filter val="6970"/>
-        <filter val="733"/>
-        <filter val="81"/>
+        <filter val="SunSpider"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added figure 8. Removed inred in intro and motivation.
</commit_message>
<xml_diff>
--- a/paper/pldi21/img/figure1.xlsx
+++ b/paper/pldi21/img/figure1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonyoungpark/Work/safe/paper/pldi21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3782834F-0DF4-5044-890E-0803F71EF689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF561798-E085-5D4D-8D72-75F88FCE61E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26660" xr2:uid="{8A9D149F-BF0C-F247-A8AE-6DB769120710}"/>
   </bookViews>
@@ -216,6 +216,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -260,9 +263,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1347,15 +1351,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>423853</xdr:colOff>
+      <xdr:colOff>423856</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>153628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4291371</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>122903</xdr:rowOff>
+      <xdr:colOff>3578225</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>111553</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1689,8 +1693,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1704,6 +1708,7 @@
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2530,7 +2535,7 @@
       </c>
     </row>
     <row r="39" spans="15:15">
-      <c r="O39">
+      <c r="O39" s="2">
         <f>AVERAGE(O26:O37)</f>
         <v>34.827013039248079</v>
       </c>

</xml_diff>

<commit_message>
Removed floating points in Figure 1.
</commit_message>
<xml_diff>
--- a/paper/pldi21/img/figure1.xlsx
+++ b/paper/pldi21/img/figure1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonyoungpark/Work/safe/paper/pldi21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEAB778-333A-894B-9940-8B2244C3D39B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A5A2E2-0C27-3347-9971-691398DD0C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26660" xr2:uid="{8A9D149F-BF0C-F247-A8AE-6DB769120710}"/>
   </bookViews>
@@ -684,7 +684,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1694,7 +1694,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G25" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>